<commit_message>
New NodeMCU AZDelivery is crap!!
</commit_message>
<xml_diff>
--- a/BOM/Teileliste.xlsx
+++ b/BOM/Teileliste.xlsx
@@ -345,9 +345,6 @@
     <t>https://www.reichelt.de/einbaubuchse-aussen-6-3-mm-innen-2-1-mm-dc-bu-072759-p208065.html?&amp;trstct=pos_7</t>
   </si>
   <si>
-    <t>https://www.amazon.de/AZDelivery-NodeMCU-ESP8266-ESP-12E-Development/dp/B06Y1LZLLY/ref=sr_1_6?s=computers&amp;ie=UTF8&amp;qid=1536349567&amp;sr=1-6&amp;keywords=esp8266</t>
-  </si>
-  <si>
     <t>Gesamt</t>
   </si>
   <si>
@@ -382,6 +379,9 @@
   </si>
   <si>
     <t>2,54 mm Raster</t>
+  </si>
+  <si>
+    <t>https://www.amazon.de/gp/product/B018E741G4/ref=oh_aui_search_detailpage?ie=UTF8&amp;psc=1</t>
   </si>
 </sst>
 </file>
@@ -723,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,7 +856,7 @@
         <v>6.99</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -906,7 +906,7 @@
         <v>90</v>
       </c>
       <c r="B9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C9">
         <v>4</v>
@@ -919,7 +919,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -969,7 +969,7 @@
         <v>93</v>
       </c>
       <c r="B12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -1008,10 +1008,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C14">
         <v>4</v>
@@ -1024,7 +1024,7 @@
         <v>4.5199999999999996</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1032,7 +1032,7 @@
         <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1045,15 +1045,15 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C16">
         <v>3</v>
@@ -1066,12 +1066,12 @@
         <v>0.75</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E18" s="2">
         <f>SUM(E2:E16)</f>
@@ -1089,12 +1089,11 @@
     <hyperlink ref="F13" r:id="rId7"/>
     <hyperlink ref="F10" r:id="rId8"/>
     <hyperlink ref="F8" r:id="rId9"/>
-    <hyperlink ref="F6" r:id="rId10"/>
-    <hyperlink ref="F15" r:id="rId11"/>
-    <hyperlink ref="F16" r:id="rId12"/>
+    <hyperlink ref="F15" r:id="rId10"/>
+    <hyperlink ref="F16" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="261" orientation="landscape" horizontalDpi="180" verticalDpi="180" r:id="rId13"/>
+  <pageSetup paperSize="261" orientation="landscape" horizontalDpi="180" verticalDpi="180" r:id="rId12"/>
 </worksheet>
 </file>
 

</xml_diff>